<commit_message>
sample contact list xlsx file
</commit_message>
<xml_diff>
--- a/assets/sample_files/Contact List.xlsx
+++ b/assets/sample_files/Contact List.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp\www\tiles\assets\sample_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27838EFF-885A-4A91-822B-4CB390192801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Contact List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -61,9 +55,6 @@
     <t>Mr. test</t>
   </si>
   <si>
-    <t>Flexible Rate=0</t>
-  </si>
-  <si>
     <t>Cash=1</t>
   </si>
   <si>
@@ -71,12 +62,15 @@
   </si>
   <si>
     <t>Walkin=3</t>
+  </si>
+  <si>
+    <t>Flexible Rate=4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -218,7 +212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -270,7 +264,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -464,18 +458,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -561,24 +555,24 @@
     </row>
     <row r="5" spans="1:13">
       <c r="K5" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="K6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="D7" s="4"/>
       <c r="K7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="D8" s="4"/>
       <c r="K8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -674,7 +668,7 @@
     <mergeCell ref="J4:M4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{53A2AE89-28D3-442B-BE0C-203186BE2D67}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>